<commit_message>
added raw region columns
</commit_message>
<xml_diff>
--- a/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
+++ b/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28308"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19540" tabRatio="971" firstSheet="7" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19540" tabRatio="971" firstSheet="7" activeTab="18"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="955" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="257">
   <si>
     <t>UK</t>
   </si>
@@ -1391,7 +1391,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1401,8 +1401,22 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="181">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1"/>
@@ -1777,7 +1791,6 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1877,9 +1890,23 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="20">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2260,7 +2287,7 @@
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
-      <c r="K2" s="156" t="s">
+      <c r="K2" s="155" t="s">
         <v>256</v>
       </c>
     </row>
@@ -2738,26 +2765,26 @@
       <c r="G53" s="1"/>
     </row>
     <row r="54" spans="2:7">
-      <c r="B54" s="155" t="s">
+      <c r="B54" s="154" t="s">
         <v>251</v>
       </c>
-      <c r="C54" s="155"/>
-      <c r="D54" s="155"/>
-      <c r="E54" s="155" t="s">
+      <c r="C54" s="154"/>
+      <c r="D54" s="154"/>
+      <c r="E54" s="154" t="s">
         <v>178</v>
       </c>
-      <c r="F54" s="155"/>
+      <c r="F54" s="154"/>
     </row>
     <row r="55" spans="2:7">
-      <c r="B55" s="155" t="s">
+      <c r="B55" s="154" t="s">
         <v>252</v>
       </c>
-      <c r="C55" s="155"/>
-      <c r="D55" s="155"/>
-      <c r="E55" s="155" t="s">
+      <c r="C55" s="154"/>
+      <c r="D55" s="154"/>
+      <c r="E55" s="154" t="s">
         <v>253</v>
       </c>
-      <c r="F55" s="155"/>
+      <c r="F55" s="154"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3015,7 +3042,7 @@
       <c r="B19" s="51">
         <v>93</v>
       </c>
-      <c r="C19" s="152">
+      <c r="C19" s="151">
         <v>100</v>
       </c>
     </row>
@@ -3152,18 +3179,18 @@
     <row r="5" spans="1:11" ht="15" thickBot="1"/>
     <row r="6" spans="1:11" ht="16" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3181,8 +3208,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:11" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -3516,7 +3543,7 @@
       <c r="F20" s="51">
         <v>586</v>
       </c>
-      <c r="G20" s="152">
+      <c r="G20" s="151">
         <v>100</v>
       </c>
       <c r="I20" s="35"/>
@@ -3843,7 +3870,7 @@
       <c r="B19" s="51">
         <v>176</v>
       </c>
-      <c r="C19" s="152">
+      <c r="C19" s="151">
         <v>100</v>
       </c>
     </row>
@@ -4010,74 +4037,74 @@
       <c r="X5" s="135"/>
     </row>
     <row r="6" spans="1:24" ht="42.5" customHeight="1">
-      <c r="A6" s="168" t="s">
+      <c r="A6" s="167" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="168"/>
-      <c r="C6" s="166" t="s">
+      <c r="B6" s="167"/>
+      <c r="C6" s="165" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="166" t="s">
+      <c r="D6" s="165" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="166" t="s">
+      <c r="E6" s="165" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="166" t="s">
+      <c r="F6" s="165" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="166" t="s">
+      <c r="G6" s="165" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="166" t="s">
+      <c r="H6" s="165" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="166" t="s">
+      <c r="I6" s="165" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="166" t="s">
+      <c r="J6" s="165" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="166" t="s">
+      <c r="K6" s="165" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="170"/>
-      <c r="O6" s="170"/>
-      <c r="P6" s="171"/>
-      <c r="Q6" s="171"/>
-      <c r="R6" s="171"/>
-      <c r="S6" s="171"/>
-      <c r="T6" s="171"/>
-      <c r="U6" s="171"/>
-      <c r="V6" s="171"/>
-      <c r="W6" s="171"/>
-      <c r="X6" s="171"/>
+      <c r="N6" s="169"/>
+      <c r="O6" s="169"/>
+      <c r="P6" s="170"/>
+      <c r="Q6" s="170"/>
+      <c r="R6" s="170"/>
+      <c r="S6" s="170"/>
+      <c r="T6" s="170"/>
+      <c r="U6" s="170"/>
+      <c r="V6" s="170"/>
+      <c r="W6" s="170"/>
+      <c r="X6" s="170"/>
     </row>
     <row r="7" spans="1:24" ht="21" customHeight="1" thickBot="1">
-      <c r="A7" s="169"/>
-      <c r="B7" s="169"/>
-      <c r="C7" s="167"/>
-      <c r="D7" s="167"/>
-      <c r="E7" s="167"/>
-      <c r="F7" s="167"/>
-      <c r="G7" s="167"/>
-      <c r="H7" s="167"/>
-      <c r="I7" s="167"/>
-      <c r="J7" s="167"/>
-      <c r="K7" s="167"/>
+      <c r="A7" s="168"/>
+      <c r="B7" s="168"/>
+      <c r="C7" s="166"/>
+      <c r="D7" s="166"/>
+      <c r="E7" s="166"/>
+      <c r="F7" s="166"/>
+      <c r="G7" s="166"/>
+      <c r="H7" s="166"/>
+      <c r="I7" s="166"/>
+      <c r="J7" s="166"/>
+      <c r="K7" s="166"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
-      <c r="N7" s="170"/>
-      <c r="O7" s="170"/>
-      <c r="P7" s="171"/>
-      <c r="Q7" s="171"/>
-      <c r="R7" s="171"/>
-      <c r="S7" s="171"/>
-      <c r="T7" s="171"/>
-      <c r="U7" s="171"/>
-      <c r="V7" s="171"/>
-      <c r="W7" s="171"/>
-      <c r="X7" s="171"/>
+      <c r="N7" s="169"/>
+      <c r="O7" s="169"/>
+      <c r="P7" s="170"/>
+      <c r="Q7" s="170"/>
+      <c r="R7" s="170"/>
+      <c r="S7" s="170"/>
+      <c r="T7" s="170"/>
+      <c r="U7" s="170"/>
+      <c r="V7" s="170"/>
+      <c r="W7" s="170"/>
+      <c r="X7" s="170"/>
     </row>
     <row r="8" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="61" t="s">
@@ -4116,7 +4143,7 @@
       <c r="L8" s="35"/>
       <c r="M8" s="35"/>
       <c r="N8" s="136"/>
-      <c r="O8" s="146"/>
+      <c r="O8" s="145"/>
       <c r="P8" s="138"/>
       <c r="Q8" s="138"/>
       <c r="R8" s="138"/>
@@ -4162,7 +4189,7 @@
       <c r="L9" s="35"/>
       <c r="M9" s="35"/>
       <c r="N9" s="139"/>
-      <c r="O9" s="146"/>
+      <c r="O9" s="145"/>
       <c r="P9" s="138"/>
       <c r="Q9" s="138"/>
       <c r="R9" s="138"/>
@@ -4178,7 +4205,7 @@
       <c r="B10" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="153">
+      <c r="C10" s="152">
         <v>829</v>
       </c>
       <c r="D10" s="68">
@@ -4222,7 +4249,7 @@
     <row r="11" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A11" s="65"/>
       <c r="B11" s="65"/>
-      <c r="C11" s="153"/>
+      <c r="C11" s="152"/>
       <c r="D11" s="69"/>
       <c r="E11" s="69"/>
       <c r="F11" s="69"/>
@@ -4344,7 +4371,7 @@
       <c r="B14" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C14" s="153">
+      <c r="C14" s="152">
         <v>36</v>
       </c>
       <c r="D14" s="68">
@@ -4388,7 +4415,7 @@
     <row r="15" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="65"/>
       <c r="B15" s="65"/>
-      <c r="C15" s="153"/>
+      <c r="C15" s="152"/>
       <c r="D15" s="69"/>
       <c r="E15" s="69"/>
       <c r="F15" s="69"/>
@@ -4508,7 +4535,7 @@
       <c r="B18" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C18" s="153">
+      <c r="C18" s="152">
         <v>26</v>
       </c>
       <c r="D18" s="68">
@@ -4550,7 +4577,7 @@
     <row r="19" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A19" s="65"/>
       <c r="B19" s="65"/>
-      <c r="C19" s="153"/>
+      <c r="C19" s="152"/>
       <c r="D19" s="69"/>
       <c r="E19" s="69"/>
       <c r="F19" s="69"/>
@@ -4666,7 +4693,7 @@
       <c r="B22" s="65" t="s">
         <v>49</v>
       </c>
-      <c r="C22" s="153">
+      <c r="C22" s="152">
         <v>891</v>
       </c>
       <c r="D22" s="68">
@@ -4739,18 +4766,18 @@
       </c>
     </row>
     <row r="28" spans="1:24" ht="29.75" customHeight="1">
-      <c r="A28" s="157" t="s">
+      <c r="A28" s="156" t="s">
         <v>246</v>
       </c>
-      <c r="B28" s="157"/>
-      <c r="C28" s="157"/>
-      <c r="D28" s="157"/>
-      <c r="E28" s="157"/>
-      <c r="F28" s="157"/>
-      <c r="G28" s="157"/>
-      <c r="H28" s="157"/>
-      <c r="I28" s="157"/>
-      <c r="J28" s="157"/>
+      <c r="B28" s="156"/>
+      <c r="C28" s="156"/>
+      <c r="D28" s="156"/>
+      <c r="E28" s="156"/>
+      <c r="F28" s="156"/>
+      <c r="G28" s="156"/>
+      <c r="H28" s="156"/>
+      <c r="I28" s="156"/>
+      <c r="J28" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -4795,7 +4822,7 @@
   <dimension ref="A1:R26"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -4857,68 +4884,68 @@
       <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:18" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B6" s="176" t="s">
+      <c r="B6" s="175" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="176"/>
-      <c r="D6" s="176"/>
-      <c r="E6" s="176"/>
-      <c r="F6" s="176"/>
-      <c r="G6" s="176" t="s">
+      <c r="C6" s="175"/>
+      <c r="D6" s="175"/>
+      <c r="E6" s="175"/>
+      <c r="F6" s="175"/>
+      <c r="G6" s="175" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="176"/>
-      <c r="I6" s="176"/>
-      <c r="J6" s="176"/>
-      <c r="K6" s="176"/>
-      <c r="L6" s="176" t="s">
+      <c r="H6" s="175"/>
+      <c r="I6" s="175"/>
+      <c r="J6" s="175"/>
+      <c r="K6" s="175"/>
+      <c r="L6" s="175" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="176"/>
-      <c r="N6" s="176"/>
-      <c r="O6" s="176"/>
-      <c r="P6" s="176"/>
+      <c r="M6" s="175"/>
+      <c r="N6" s="175"/>
+      <c r="O6" s="175"/>
+      <c r="P6" s="175"/>
     </row>
     <row r="7" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="177" t="s">
+      <c r="A7" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="172" t="s">
+      <c r="B7" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="172"/>
-      <c r="D7" s="172" t="s">
+      <c r="C7" s="171"/>
+      <c r="D7" s="171" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="172"/>
-      <c r="F7" s="173" t="s">
+      <c r="E7" s="171"/>
+      <c r="F7" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="172" t="s">
+      <c r="G7" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="172"/>
-      <c r="I7" s="172" t="s">
+      <c r="H7" s="171"/>
+      <c r="I7" s="171" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="172"/>
-      <c r="K7" s="173" t="s">
+      <c r="J7" s="171"/>
+      <c r="K7" s="172" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="172" t="s">
+      <c r="L7" s="171" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="172"/>
-      <c r="N7" s="172" t="s">
+      <c r="M7" s="171"/>
+      <c r="N7" s="171" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="172"/>
-      <c r="P7" s="173" t="s">
+      <c r="O7" s="171"/>
+      <c r="P7" s="172" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="178"/>
+      <c r="A8" s="177"/>
       <c r="B8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4931,7 +4958,7 @@
       <c r="E8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="174"/>
+      <c r="F8" s="173"/>
       <c r="G8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4944,7 +4971,7 @@
       <c r="J8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="174"/>
+      <c r="K8" s="173"/>
       <c r="L8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4957,7 +4984,7 @@
       <c r="O8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="174"/>
+      <c r="P8" s="173"/>
     </row>
     <row r="9" spans="1:18" ht="21" customHeight="1" thickTop="1">
       <c r="A9" s="87" t="s">
@@ -5432,15 +5459,15 @@
       <c r="H19" s="83"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="175" t="s">
+      <c r="A20" s="174" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="175"/>
-      <c r="C20" s="175"/>
-      <c r="D20" s="175"/>
-      <c r="E20" s="175"/>
-      <c r="F20" s="175"/>
-      <c r="G20" s="175"/>
+      <c r="B20" s="174"/>
+      <c r="C20" s="174"/>
+      <c r="D20" s="174"/>
+      <c r="E20" s="174"/>
+      <c r="F20" s="174"/>
+      <c r="G20" s="174"/>
       <c r="H20" s="83"/>
     </row>
     <row r="21" spans="1:18">
@@ -5492,18 +5519,18 @@
       <c r="H24" s="83"/>
     </row>
     <row r="25" spans="1:18" ht="31.5" customHeight="1">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="157"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="82"/>
@@ -5594,18 +5621,18 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="178" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="178" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="179"/>
-      <c r="F6" s="173" t="s">
+      <c r="E6" s="178"/>
+      <c r="F6" s="172" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="77" t="s">
@@ -5613,7 +5640,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="178"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="124" t="s">
         <v>20</v>
       </c>
@@ -5626,7 +5653,7 @@
       <c r="E7" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="174"/>
+      <c r="F7" s="173"/>
     </row>
     <row r="8" spans="1:23" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="87" t="s">
@@ -5834,14 +5861,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="175" t="s">
+      <c r="A19" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -5884,18 +5911,18 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="30.5" customHeight="1">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -5927,7 +5954,7 @@
   <sheetPr codeName="Sheet15" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -5986,33 +6013,33 @@
       <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="180"/>
-      <c r="D6" s="180"/>
-      <c r="E6" s="180"/>
-      <c r="F6" s="180"/>
-      <c r="G6" s="180" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="179"/>
+      <c r="E6" s="179"/>
+      <c r="F6" s="179"/>
+      <c r="G6" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="180"/>
-      <c r="I6" s="180"/>
-      <c r="J6" s="180"/>
-      <c r="K6" s="180"/>
-      <c r="L6" s="180" t="s">
+      <c r="H6" s="179"/>
+      <c r="I6" s="179"/>
+      <c r="J6" s="179"/>
+      <c r="K6" s="179"/>
+      <c r="L6" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="180"/>
-      <c r="N6" s="180"/>
-      <c r="O6" s="180"/>
-      <c r="P6" s="180"/>
+      <c r="M6" s="179"/>
+      <c r="N6" s="179"/>
+      <c r="O6" s="179"/>
+      <c r="P6" s="179"/>
     </row>
     <row r="7" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="178"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="96" t="s">
         <v>79</v>
       </c>
@@ -6524,15 +6551,15 @@
       <c r="H18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="175" t="s">
+      <c r="A19" s="174" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
-      <c r="G19" s="175"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
+      <c r="G19" s="174"/>
       <c r="H19" s="83"/>
     </row>
     <row r="20" spans="1:10">
@@ -6584,18 +6611,18 @@
       <c r="H23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="27" customHeight="1">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -6625,9 +6652,11 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:S29"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -6642,7 +6671,7 @@
     <col min="9" max="16384" width="8.83203125" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:19">
       <c r="A1" s="76" t="s">
         <v>208</v>
       </c>
@@ -6650,22 +6679,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:19">
       <c r="A2" s="76" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:19">
       <c r="A3" s="76" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:19">
       <c r="A4" s="76" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="14" thickBot="1">
+    <row r="5" spans="1:19" ht="14" thickBot="1">
       <c r="A5" s="79"/>
       <c r="B5" s="80"/>
       <c r="C5" s="80"/>
@@ -6675,7 +6704,7 @@
       <c r="G5" s="80"/>
       <c r="H5" s="80"/>
     </row>
-    <row r="6" spans="1:12" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="6" spans="1:19" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="101" t="s">
         <v>1</v>
       </c>
@@ -6701,7 +6730,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="21" customHeight="1" thickTop="1">
+    <row r="7" spans="1:19" ht="21" customHeight="1" thickTop="1">
       <c r="A7" s="87" t="s">
         <v>222</v>
       </c>
@@ -6709,13 +6738,13 @@
         <v>442</v>
       </c>
       <c r="C7" s="98">
-        <v>101.8</v>
+        <v>102</v>
       </c>
       <c r="D7" s="98">
-        <v>166.8</v>
+        <v>167</v>
       </c>
       <c r="E7" s="98">
-        <v>119.3</v>
+        <v>119</v>
       </c>
       <c r="F7" s="98">
         <v>39</v>
@@ -6724,155 +6753,190 @@
         <v>16</v>
       </c>
       <c r="H7" s="98">
-        <v>891.4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="21" customHeight="1">
+        <v>891</v>
+      </c>
+      <c r="J7" s="144"/>
+      <c r="K7" s="144"/>
+      <c r="L7" s="144"/>
+      <c r="Q7" s="144"/>
+      <c r="R7" s="144"/>
+      <c r="S7" s="144"/>
+    </row>
+    <row r="8" spans="1:19" ht="21" customHeight="1">
       <c r="A8" s="84" t="s">
         <v>2</v>
       </c>
       <c r="B8" s="97">
-        <v>1206.3</v>
+        <v>1206</v>
       </c>
       <c r="C8" s="97">
-        <v>171.2</v>
+        <v>171</v>
       </c>
       <c r="D8" s="97">
         <v>284</v>
       </c>
       <c r="E8" s="97">
-        <v>188.7</v>
+        <v>189</v>
       </c>
       <c r="F8" s="97">
-        <v>58.2</v>
+        <v>58</v>
       </c>
       <c r="G8" s="97">
-        <v>32.799999999999997</v>
+        <v>33</v>
       </c>
       <c r="H8" s="97">
-        <v>1958.3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="21" customHeight="1">
+        <v>1958</v>
+      </c>
+      <c r="J8" s="144"/>
+      <c r="K8" s="144"/>
+      <c r="L8" s="144"/>
+      <c r="Q8" s="144"/>
+      <c r="R8" s="144"/>
+      <c r="S8" s="144"/>
+    </row>
+    <row r="9" spans="1:19" ht="21" customHeight="1">
       <c r="A9" s="87" t="s">
         <v>3</v>
       </c>
       <c r="B9" s="98">
-        <v>384.7</v>
+        <v>385</v>
       </c>
       <c r="C9" s="98">
-        <v>64.7</v>
+        <v>65</v>
       </c>
       <c r="D9" s="98">
-        <v>100.5</v>
+        <v>101</v>
       </c>
       <c r="E9" s="98">
-        <v>71.900000000000006</v>
+        <v>72</v>
       </c>
       <c r="F9" s="98">
-        <v>17.899999999999999</v>
+        <v>18</v>
       </c>
       <c r="G9" s="98" t="s">
         <v>22</v>
       </c>
       <c r="H9" s="98">
-        <v>653.9</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="21" customHeight="1">
+        <v>654</v>
+      </c>
+      <c r="J9" s="144"/>
+      <c r="K9" s="144"/>
+      <c r="L9" s="144"/>
+      <c r="Q9" s="144"/>
+      <c r="R9" s="144"/>
+      <c r="S9" s="144"/>
+    </row>
+    <row r="10" spans="1:19" ht="21" customHeight="1">
       <c r="A10" s="87" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="98">
-        <v>814.2</v>
+        <v>814</v>
       </c>
       <c r="C10" s="98">
-        <v>129.30000000000001</v>
+        <v>129</v>
       </c>
       <c r="D10" s="98">
-        <v>254.2</v>
+        <v>254</v>
       </c>
       <c r="E10" s="98">
-        <v>164.7</v>
+        <v>165</v>
       </c>
       <c r="F10" s="98">
-        <v>47.1</v>
+        <v>47</v>
       </c>
       <c r="G10" s="98">
-        <v>26.9</v>
+        <v>27</v>
       </c>
       <c r="H10" s="98">
-        <v>1455.2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="21" customHeight="1">
+        <v>1455</v>
+      </c>
+      <c r="J10" s="144"/>
+      <c r="K10" s="144"/>
+      <c r="L10" s="144"/>
+      <c r="Q10" s="144"/>
+      <c r="R10" s="144"/>
+      <c r="S10" s="144"/>
+    </row>
+    <row r="11" spans="1:19" ht="21" customHeight="1">
       <c r="A11" s="87" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="98">
-        <v>15.2</v>
+        <v>15</v>
       </c>
       <c r="C11" s="98">
-        <v>5.5</v>
+        <v>6</v>
       </c>
       <c r="D11" s="98">
-        <v>24.5</v>
+        <v>25</v>
       </c>
       <c r="E11" s="98">
-        <v>31.3</v>
+        <v>31</v>
       </c>
       <c r="F11" s="98" t="s">
         <v>22</v>
       </c>
       <c r="G11" s="98">
-        <v>8.6999999999999993</v>
+        <v>9</v>
       </c>
       <c r="H11" s="98">
-        <v>92.9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="21" customHeight="1">
+        <v>93</v>
+      </c>
+      <c r="J11" s="144"/>
+      <c r="K11" s="144"/>
+      <c r="L11" s="144"/>
+      <c r="Q11" s="144"/>
+      <c r="R11" s="144"/>
+      <c r="S11" s="144"/>
+    </row>
+    <row r="12" spans="1:19" ht="21" customHeight="1">
       <c r="A12" s="87" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="98">
-        <v>158.80000000000001</v>
+        <v>159</v>
       </c>
       <c r="C12" s="98">
         <v>45</v>
       </c>
       <c r="D12" s="98">
-        <v>174.4</v>
+        <v>174</v>
       </c>
       <c r="E12" s="98">
-        <v>141.1</v>
+        <v>141</v>
       </c>
       <c r="F12" s="98">
-        <v>36.6</v>
+        <v>37</v>
       </c>
       <c r="G12" s="98">
-        <v>20.5</v>
+        <v>21</v>
       </c>
       <c r="H12" s="98">
         <v>586</v>
       </c>
-      <c r="L12" s="145"/>
-    </row>
-    <row r="13" spans="1:12" ht="21" customHeight="1" thickBot="1">
+      <c r="J12" s="144"/>
+      <c r="K12" s="144"/>
+      <c r="L12" s="144"/>
+      <c r="Q12" s="144"/>
+      <c r="R12" s="144"/>
+      <c r="S12" s="144"/>
+    </row>
+    <row r="13" spans="1:19" ht="21" customHeight="1" thickBot="1">
       <c r="A13" s="87" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="98">
-        <v>70.900000000000006</v>
+        <v>71</v>
       </c>
       <c r="C13" s="98">
-        <v>17.3</v>
+        <v>17</v>
       </c>
       <c r="D13" s="98">
         <v>47</v>
       </c>
       <c r="E13" s="98">
-        <v>29.4</v>
+        <v>29</v>
       </c>
       <c r="F13" s="98" t="s">
         <v>22</v>
@@ -6881,62 +6945,80 @@
         <v>22</v>
       </c>
       <c r="H13" s="98">
-        <v>176.3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" ht="23.5" customHeight="1" thickTop="1" thickBot="1">
+        <v>176</v>
+      </c>
+      <c r="J13" s="144"/>
+      <c r="K13" s="144"/>
+      <c r="L13" s="144"/>
+      <c r="Q13" s="144"/>
+      <c r="R13" s="144"/>
+      <c r="S13" s="144"/>
+    </row>
+    <row r="14" spans="1:19" ht="23.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A14" s="90" t="s">
         <v>91</v>
       </c>
       <c r="B14" s="99">
-        <v>1954.2</v>
+        <v>1954</v>
       </c>
       <c r="C14" s="99">
-        <v>363.3</v>
+        <v>363</v>
       </c>
       <c r="D14" s="99">
-        <v>746.2</v>
+        <v>746</v>
       </c>
       <c r="E14" s="99">
-        <v>546.29999999999995</v>
+        <v>546</v>
       </c>
       <c r="F14" s="99">
-        <v>158.4</v>
+        <v>158</v>
       </c>
       <c r="G14" s="99">
-        <v>88.9</v>
+        <v>89</v>
       </c>
       <c r="H14" s="99">
         <v>3901</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="J14" s="144"/>
+      <c r="K14" s="144"/>
+      <c r="L14" s="144"/>
+      <c r="Q14" s="144"/>
+      <c r="R14" s="144"/>
+      <c r="S14" s="144"/>
+    </row>
+    <row r="15" spans="1:19" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="93" t="s">
         <v>23</v>
       </c>
       <c r="B15" s="100">
-        <v>11001.2</v>
+        <v>11001</v>
       </c>
       <c r="C15" s="100">
-        <v>3095.5</v>
+        <v>3096</v>
       </c>
       <c r="D15" s="100">
-        <v>7271.1</v>
+        <v>7271</v>
       </c>
       <c r="E15" s="100">
-        <v>6186.8</v>
+        <v>6187</v>
       </c>
       <c r="F15" s="100">
-        <v>2624.8</v>
+        <v>2625</v>
       </c>
       <c r="G15" s="100">
-        <v>1668.5</v>
+        <v>1669</v>
       </c>
       <c r="H15" s="100">
-        <v>32422.400000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="14" thickTop="1"/>
+        <v>32422</v>
+      </c>
+      <c r="J15" s="144"/>
+      <c r="K15" s="144"/>
+      <c r="L15" s="144"/>
+      <c r="Q15" s="144"/>
+      <c r="R15" s="144"/>
+      <c r="S15" s="144"/>
+    </row>
+    <row r="16" spans="1:19" ht="14" thickTop="1"/>
     <row r="17" spans="1:10">
       <c r="A17" s="81" t="s">
         <v>10</v>
@@ -6950,15 +7032,15 @@
       <c r="H17" s="83"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="175" t="s">
+      <c r="A18" s="174" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="175"/>
-      <c r="C18" s="175"/>
-      <c r="D18" s="175"/>
-      <c r="E18" s="175"/>
-      <c r="F18" s="175"/>
-      <c r="G18" s="175"/>
+      <c r="B18" s="174"/>
+      <c r="C18" s="174"/>
+      <c r="D18" s="174"/>
+      <c r="E18" s="174"/>
+      <c r="F18" s="174"/>
+      <c r="G18" s="174"/>
       <c r="H18" s="83"/>
     </row>
     <row r="19" spans="1:10">
@@ -7022,18 +7104,18 @@
       <c r="H23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="25.25" customHeight="1">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="156" t="s">
         <v>249</v>
       </c>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82" t="s">
@@ -7082,7 +7164,9 @@
   <sheetPr codeName="Sheet17" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -7127,18 +7211,18 @@
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="177" t="s">
+      <c r="A6" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="178" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="178" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="179"/>
-      <c r="F6" s="173" t="s">
+      <c r="E6" s="178"/>
+      <c r="F6" s="172" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="77" t="s">
@@ -7146,7 +7230,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="178"/>
+      <c r="A7" s="177"/>
       <c r="B7" s="124" t="s">
         <v>20</v>
       </c>
@@ -7159,26 +7243,26 @@
       <c r="E7" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="174"/>
+      <c r="F7" s="173"/>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="87" t="s">
         <v>220</v>
       </c>
       <c r="B8" s="88">
-        <v>556.29999999999995</v>
+        <v>556</v>
       </c>
       <c r="C8" s="89">
         <v>62.4</v>
       </c>
       <c r="D8" s="88">
-        <v>335.1</v>
+        <v>335</v>
       </c>
       <c r="E8" s="89">
         <v>37.6</v>
       </c>
       <c r="F8" s="88">
-        <v>891.4</v>
+        <v>891</v>
       </c>
       <c r="H8" s="118"/>
       <c r="I8" s="118"/>
@@ -7194,13 +7278,13 @@
         <v>78.2</v>
       </c>
       <c r="D9" s="85">
-        <v>422.5</v>
+        <v>422</v>
       </c>
       <c r="E9" s="86">
         <v>21.6</v>
       </c>
       <c r="F9" s="85">
-        <v>1958.3</v>
+        <v>1958</v>
       </c>
       <c r="H9" s="118"/>
       <c r="I9" s="118"/>
@@ -7210,19 +7294,19 @@
         <v>3</v>
       </c>
       <c r="B10" s="88">
-        <v>441.8</v>
+        <v>442</v>
       </c>
       <c r="C10" s="89">
         <v>67.599999999999994</v>
       </c>
       <c r="D10" s="88">
-        <v>210.1</v>
+        <v>210</v>
       </c>
       <c r="E10" s="89">
         <v>32.1</v>
       </c>
       <c r="F10" s="88">
-        <v>653.9</v>
+        <v>654</v>
       </c>
       <c r="H10" s="118"/>
       <c r="I10" s="118"/>
@@ -7232,19 +7316,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="88">
-        <v>1268.5999999999999</v>
+        <v>1269</v>
       </c>
       <c r="C11" s="89">
         <v>87.2</v>
       </c>
       <c r="D11" s="88">
-        <v>185.2</v>
+        <v>185</v>
       </c>
       <c r="E11" s="89">
         <v>12.7</v>
       </c>
       <c r="F11" s="88">
-        <v>1455.2</v>
+        <v>1455</v>
       </c>
       <c r="H11" s="118"/>
       <c r="I11" s="118"/>
@@ -7254,19 +7338,19 @@
         <v>5</v>
       </c>
       <c r="B12" s="88">
-        <v>65.5</v>
+        <v>65</v>
       </c>
       <c r="C12" s="89">
         <v>70.400000000000006</v>
       </c>
       <c r="D12" s="88">
-        <v>27.5</v>
+        <v>27</v>
       </c>
       <c r="E12" s="89">
         <v>29.6</v>
       </c>
       <c r="F12" s="88">
-        <v>92.9</v>
+        <v>93</v>
       </c>
       <c r="H12" s="118"/>
       <c r="I12" s="118"/>
@@ -7276,13 +7360,13 @@
         <v>6</v>
       </c>
       <c r="B13" s="88">
-        <v>328.6</v>
+        <v>329</v>
       </c>
       <c r="C13" s="89">
         <v>56.1</v>
       </c>
       <c r="D13" s="88">
-        <v>255.7</v>
+        <v>256</v>
       </c>
       <c r="E13" s="89">
         <v>43.6</v>
@@ -7298,19 +7382,19 @@
         <v>7</v>
       </c>
       <c r="B14" s="88">
-        <v>165.3</v>
+        <v>165</v>
       </c>
       <c r="C14" s="89">
         <v>93.8</v>
       </c>
       <c r="D14" s="88">
-        <v>10.9</v>
+        <v>11</v>
       </c>
       <c r="E14" s="89">
         <v>6.2</v>
       </c>
       <c r="F14" s="88">
-        <v>176.3</v>
+        <v>176</v>
       </c>
       <c r="H14" s="118"/>
       <c r="I14" s="118"/>
@@ -7326,7 +7410,7 @@
         <v>72.900000000000006</v>
       </c>
       <c r="D15" s="91">
-        <v>1052.8</v>
+        <v>1053</v>
       </c>
       <c r="E15" s="92">
         <v>27</v>
@@ -7342,19 +7426,19 @@
         <v>23</v>
       </c>
       <c r="B16" s="94">
-        <v>23546.6</v>
+        <v>23547</v>
       </c>
       <c r="C16" s="95">
         <v>72.599999999999994</v>
       </c>
       <c r="D16" s="94">
-        <v>8836.2000000000007</v>
+        <v>8836</v>
       </c>
       <c r="E16" s="95">
         <v>27.3</v>
       </c>
       <c r="F16" s="94">
-        <v>32422.400000000001</v>
+        <v>32422</v>
       </c>
       <c r="H16" s="118"/>
       <c r="I16" s="118"/>
@@ -7371,14 +7455,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="175" t="s">
+      <c r="A19" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -7421,18 +7505,18 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="27" customHeight="1">
-      <c r="A24" s="157" t="s">
+      <c r="A24" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="157"/>
-      <c r="C24" s="157"/>
-      <c r="D24" s="157"/>
-      <c r="E24" s="157"/>
-      <c r="F24" s="157"/>
-      <c r="G24" s="157"/>
-      <c r="H24" s="157"/>
-      <c r="I24" s="157"/>
-      <c r="J24" s="157"/>
+      <c r="B24" s="156"/>
+      <c r="C24" s="156"/>
+      <c r="D24" s="156"/>
+      <c r="E24" s="156"/>
+      <c r="F24" s="156"/>
+      <c r="G24" s="156"/>
+      <c r="H24" s="156"/>
+      <c r="I24" s="156"/>
+      <c r="J24" s="156"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -7461,9 +7545,11 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J25"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
   <cols>
@@ -7479,7 +7565,7 @@
     <col min="11" max="16384" width="8.83203125" style="77"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:14">
       <c r="A1" s="76" t="s">
         <v>210</v>
       </c>
@@ -7487,22 +7573,22 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:14">
       <c r="A2" s="76" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:14">
       <c r="A3" s="76" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:14">
       <c r="A4" s="76" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="14" thickBot="1">
+    <row r="5" spans="1:14" ht="14" thickBot="1">
       <c r="A5" s="79"/>
       <c r="B5" s="121"/>
       <c r="C5" s="121"/>
@@ -7510,28 +7596,28 @@
       <c r="E5" s="121"/>
       <c r="F5" s="121"/>
     </row>
-    <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="177" t="s">
+    <row r="6" spans="1:14" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A6" s="176" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="178" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179" t="s">
+      <c r="C6" s="178"/>
+      <c r="D6" s="178" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179" t="s">
+      <c r="E6" s="178"/>
+      <c r="F6" s="178" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="179"/>
+      <c r="G6" s="178"/>
       <c r="I6" s="77" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="178"/>
+    <row r="7" spans="1:14" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A7" s="177"/>
       <c r="B7" s="124" t="s">
         <v>211</v>
       </c>
@@ -7552,32 +7638,37 @@
       </c>
       <c r="H7" s="120"/>
     </row>
-    <row r="8" spans="1:10" ht="21" customHeight="1" thickTop="1">
+    <row r="8" spans="1:14" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="87" t="s">
         <v>222</v>
       </c>
       <c r="B8" s="122">
-        <v>599.79999999999995</v>
+        <v>600</v>
       </c>
       <c r="C8" s="125">
-        <v>231.4</v>
+        <v>231</v>
       </c>
       <c r="D8" s="122">
-        <v>53.4</v>
+        <v>53</v>
       </c>
       <c r="E8" s="125">
-        <v>6.9</v>
+        <v>7</v>
       </c>
       <c r="F8" s="122">
-        <v>653.1</v>
+        <v>653</v>
       </c>
       <c r="G8" s="122">
-        <v>238.3</v>
+        <v>238</v>
       </c>
       <c r="H8" s="118"/>
       <c r="I8" s="118"/>
-    </row>
-    <row r="9" spans="1:10" ht="21" customHeight="1">
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="118"/>
+      <c r="N8" s="118"/>
+    </row>
+    <row r="9" spans="1:14" ht="21" customHeight="1">
       <c r="A9" s="84" t="s">
         <v>2</v>
       </c>
@@ -7585,113 +7676,133 @@
         <v>1145</v>
       </c>
       <c r="C9" s="126">
-        <v>138.6</v>
+        <v>139</v>
       </c>
       <c r="D9" s="85">
         <v>649</v>
       </c>
       <c r="E9" s="126">
-        <v>25.7</v>
+        <v>26</v>
       </c>
       <c r="F9" s="85">
         <v>1794</v>
       </c>
       <c r="G9" s="85">
-        <v>164.3</v>
+        <v>164</v>
       </c>
       <c r="H9" s="118"/>
       <c r="I9" s="118"/>
-    </row>
-    <row r="10" spans="1:10" ht="21" customHeight="1">
+      <c r="J9" s="118"/>
+      <c r="K9" s="118"/>
+      <c r="L9" s="118"/>
+      <c r="M9" s="118"/>
+      <c r="N9" s="118"/>
+    </row>
+    <row r="10" spans="1:14" ht="21" customHeight="1">
       <c r="A10" s="87" t="s">
         <v>3</v>
       </c>
       <c r="B10" s="88">
-        <v>269.10000000000002</v>
+        <v>269</v>
       </c>
       <c r="C10" s="127">
-        <v>73.400000000000006</v>
+        <v>73</v>
       </c>
       <c r="D10" s="88">
         <v>296</v>
       </c>
       <c r="E10" s="127">
-        <v>15.3</v>
+        <v>15</v>
       </c>
       <c r="F10" s="88">
-        <v>565.1</v>
+        <v>565</v>
       </c>
       <c r="G10" s="88">
-        <v>88.8</v>
+        <v>89</v>
       </c>
       <c r="H10" s="118"/>
       <c r="I10" s="118"/>
-    </row>
-    <row r="11" spans="1:10" ht="21" customHeight="1">
+      <c r="J10" s="118"/>
+      <c r="K10" s="118"/>
+      <c r="L10" s="118"/>
+      <c r="M10" s="118"/>
+      <c r="N10" s="118"/>
+    </row>
+    <row r="11" spans="1:14" ht="21" customHeight="1">
       <c r="A11" s="87" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="88">
-        <v>1071.7</v>
+        <v>1072</v>
       </c>
       <c r="C11" s="127">
         <v>121</v>
       </c>
       <c r="D11" s="88">
-        <v>255.5</v>
+        <v>256</v>
       </c>
       <c r="E11" s="127">
         <v>7</v>
       </c>
       <c r="F11" s="88">
-        <v>1327.2</v>
+        <v>1327</v>
       </c>
       <c r="G11" s="88">
         <v>128</v>
       </c>
       <c r="H11" s="118"/>
       <c r="I11" s="118"/>
-    </row>
-    <row r="12" spans="1:10" ht="21" customHeight="1">
+      <c r="J11" s="118"/>
+      <c r="K11" s="118"/>
+      <c r="L11" s="118"/>
+      <c r="M11" s="118"/>
+      <c r="N11" s="118"/>
+    </row>
+    <row r="12" spans="1:14" ht="21" customHeight="1">
       <c r="A12" s="87" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="88" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="127" t="s">
-        <v>22</v>
-      </c>
-      <c r="D12" s="88" t="s">
-        <v>22</v>
+      <c r="B12" s="88">
+        <v>0</v>
+      </c>
+      <c r="C12" s="127">
+        <v>0</v>
+      </c>
+      <c r="D12" s="88">
+        <v>0</v>
       </c>
       <c r="E12" s="127">
         <v>0</v>
       </c>
       <c r="F12" s="88">
-        <v>69.099999999999994</v>
+        <v>69</v>
       </c>
       <c r="G12" s="88">
-        <v>23.9</v>
+        <v>24</v>
       </c>
       <c r="H12" s="118"/>
       <c r="I12" s="118"/>
-    </row>
-    <row r="13" spans="1:10" ht="21" customHeight="1">
+      <c r="J12" s="118"/>
+      <c r="K12" s="118"/>
+      <c r="L12" s="118"/>
+      <c r="M12" s="118"/>
+      <c r="N12" s="118"/>
+    </row>
+    <row r="13" spans="1:14" ht="21" customHeight="1">
       <c r="A13" s="87" t="s">
         <v>6</v>
       </c>
       <c r="B13" s="88">
-        <v>211.6</v>
+        <v>212</v>
       </c>
       <c r="C13" s="127">
-        <v>249.7</v>
+        <v>250</v>
       </c>
       <c r="D13" s="88">
-        <v>113.3</v>
+        <v>113</v>
       </c>
       <c r="E13" s="127">
-        <v>11.3</v>
+        <v>11</v>
       </c>
       <c r="F13" s="88">
         <v>325</v>
@@ -7701,82 +7812,101 @@
       </c>
       <c r="H13" s="118"/>
       <c r="I13" s="118"/>
-    </row>
-    <row r="14" spans="1:10" ht="21" customHeight="1" thickBot="1">
+      <c r="J13" s="118"/>
+      <c r="K13" s="118"/>
+      <c r="L13" s="118"/>
+      <c r="M13" s="118"/>
+      <c r="N13" s="118"/>
+    </row>
+    <row r="14" spans="1:14" ht="21" customHeight="1" thickBot="1">
       <c r="A14" s="87" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="88" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="127" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="88" t="s">
-        <v>22</v>
-      </c>
-      <c r="E14" s="127" t="s">
-        <v>22</v>
+      <c r="B14" s="88">
+        <v>0</v>
+      </c>
+      <c r="C14" s="127">
+        <v>0</v>
+      </c>
+      <c r="D14" s="88">
+        <v>0</v>
+      </c>
+      <c r="E14" s="127">
+        <v>0</v>
       </c>
       <c r="F14" s="88">
-        <v>156.9</v>
+        <v>157</v>
       </c>
       <c r="G14" s="88">
-        <v>19.399999999999999</v>
+        <v>19</v>
       </c>
       <c r="H14" s="118"/>
       <c r="I14" s="118"/>
-    </row>
-    <row r="15" spans="1:10" ht="23.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="J14" s="118"/>
+      <c r="K14" s="118"/>
+      <c r="L14" s="118"/>
+      <c r="M14" s="118"/>
+      <c r="N14" s="118"/>
+    </row>
+    <row r="15" spans="1:14" ht="23.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A15" s="90" t="s">
         <v>91</v>
       </c>
       <c r="B15" s="91">
-        <v>2317.6</v>
+        <v>2318</v>
       </c>
       <c r="C15" s="128">
-        <v>693.7</v>
+        <v>694</v>
       </c>
       <c r="D15" s="91">
-        <v>846.2</v>
+        <v>846</v>
       </c>
       <c r="E15" s="128">
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="F15" s="91">
-        <v>3163.8</v>
+        <v>3164</v>
       </c>
       <c r="G15" s="91">
-        <v>737.3</v>
+        <v>737</v>
       </c>
       <c r="H15" s="118"/>
       <c r="I15" s="118"/>
-      <c r="J15" s="144"/>
-    </row>
-    <row r="16" spans="1:10" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="118"/>
+      <c r="N15" s="118"/>
+    </row>
+    <row r="16" spans="1:14" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A16" s="93" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="129">
-        <v>16548.8</v>
+        <v>16549</v>
       </c>
       <c r="C16" s="130">
-        <v>10602.3</v>
+        <v>10602</v>
       </c>
       <c r="D16" s="129">
-        <v>5130.3999999999996</v>
+        <v>5130</v>
       </c>
       <c r="E16" s="130">
-        <v>140.80000000000001</v>
+        <v>141</v>
       </c>
       <c r="F16" s="129">
-        <v>21679.200000000001</v>
+        <v>21679</v>
       </c>
       <c r="G16" s="129">
-        <v>10743.2</v>
+        <v>10743</v>
       </c>
       <c r="H16" s="118"/>
       <c r="I16" s="118"/>
+      <c r="J16" s="118"/>
+      <c r="K16" s="118"/>
+      <c r="L16" s="118"/>
+      <c r="M16" s="118"/>
+      <c r="N16" s="118"/>
     </row>
     <row r="17" spans="1:10" ht="14" thickTop="1"/>
     <row r="18" spans="1:10">
@@ -7790,14 +7920,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="175" t="s">
+      <c r="A19" s="174" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="175"/>
-      <c r="C19" s="175"/>
-      <c r="D19" s="175"/>
-      <c r="E19" s="175"/>
-      <c r="F19" s="175"/>
+      <c r="B19" s="174"/>
+      <c r="C19" s="174"/>
+      <c r="D19" s="174"/>
+      <c r="E19" s="174"/>
+      <c r="F19" s="174"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -7840,29 +7970,29 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A24" s="175" t="s">
+      <c r="A24" s="174" t="s">
         <v>217</v>
       </c>
-      <c r="B24" s="175"/>
-      <c r="C24" s="175"/>
-      <c r="D24" s="175"/>
-      <c r="E24" s="175"/>
-      <c r="F24" s="175"/>
-      <c r="G24" s="175"/>
+      <c r="B24" s="174"/>
+      <c r="C24" s="174"/>
+      <c r="D24" s="174"/>
+      <c r="E24" s="174"/>
+      <c r="F24" s="174"/>
+      <c r="G24" s="174"/>
     </row>
     <row r="25" spans="1:10" ht="17.75" customHeight="1">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="156" t="s">
         <v>249</v>
       </c>
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="157"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8381,18 +8511,18 @@
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:13" ht="29.25" customHeight="1">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="156" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
+      <c r="H21" s="156"/>
+      <c r="I21" s="156"/>
+      <c r="J21" s="156"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
@@ -8437,18 +8567,18 @@
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="28.5" customHeight="1">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="157"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="5" t="s">
@@ -9720,15 +9850,15 @@
       <c r="G77" s="83"/>
     </row>
     <row r="78" spans="1:7" ht="27.5" customHeight="1">
-      <c r="A78" s="175" t="s">
+      <c r="A78" s="174" t="s">
         <v>250</v>
       </c>
-      <c r="B78" s="175"/>
-      <c r="C78" s="175"/>
-      <c r="D78" s="175"/>
-      <c r="E78" s="175"/>
-      <c r="F78" s="175"/>
-      <c r="G78" s="175"/>
+      <c r="B78" s="174"/>
+      <c r="C78" s="174"/>
+      <c r="D78" s="174"/>
+      <c r="E78" s="174"/>
+      <c r="F78" s="174"/>
+      <c r="G78" s="174"/>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="82" t="s">
@@ -9775,18 +9905,18 @@
       <c r="G82" s="83"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="157" t="s">
+      <c r="A83" s="156" t="s">
         <v>245</v>
       </c>
-      <c r="B83" s="157"/>
-      <c r="C83" s="157"/>
-      <c r="D83" s="157"/>
-      <c r="E83" s="157"/>
-      <c r="F83" s="157"/>
-      <c r="G83" s="157"/>
-      <c r="H83" s="157"/>
-      <c r="I83" s="157"/>
-      <c r="J83" s="157"/>
+      <c r="B83" s="156"/>
+      <c r="C83" s="156"/>
+      <c r="D83" s="156"/>
+      <c r="E83" s="156"/>
+      <c r="F83" s="156"/>
+      <c r="G83" s="156"/>
+      <c r="H83" s="156"/>
+      <c r="I83" s="156"/>
+      <c r="J83" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10262,18 +10392,18 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" ht="26.75" customHeight="1">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="156" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="157"/>
-      <c r="C21" s="157"/>
-      <c r="D21" s="157"/>
-      <c r="E21" s="157"/>
-      <c r="F21" s="157"/>
-      <c r="G21" s="157"/>
-      <c r="H21" s="157"/>
-      <c r="I21" s="157"/>
-      <c r="J21" s="157"/>
+      <c r="B21" s="156"/>
+      <c r="C21" s="156"/>
+      <c r="D21" s="156"/>
+      <c r="E21" s="156"/>
+      <c r="F21" s="156"/>
+      <c r="G21" s="156"/>
+      <c r="H21" s="156"/>
+      <c r="I21" s="156"/>
+      <c r="J21" s="156"/>
       <c r="L21" s="32"/>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
@@ -10282,18 +10412,18 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" ht="29.25" customHeight="1">
-      <c r="A22" s="157" t="s">
+      <c r="A22" s="156" t="s">
         <v>244</v>
       </c>
-      <c r="B22" s="157"/>
-      <c r="C22" s="157"/>
-      <c r="D22" s="157"/>
-      <c r="E22" s="157"/>
-      <c r="F22" s="157"/>
-      <c r="G22" s="157"/>
-      <c r="H22" s="157"/>
-      <c r="I22" s="157"/>
-      <c r="J22" s="157"/>
+      <c r="B22" s="156"/>
+      <c r="C22" s="156"/>
+      <c r="D22" s="156"/>
+      <c r="E22" s="156"/>
+      <c r="F22" s="156"/>
+      <c r="G22" s="156"/>
+      <c r="H22" s="156"/>
+      <c r="I22" s="156"/>
+      <c r="J22" s="156"/>
       <c r="L22" s="32"/>
       <c r="M22" s="32"/>
       <c r="N22" s="32"/>
@@ -10465,36 +10595,36 @@
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1"/>
     <row r="6" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="161" t="s">
+      <c r="A6" s="160" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="158" t="s">
+      <c r="B6" s="157" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="158"/>
-      <c r="D6" s="158" t="s">
+      <c r="C6" s="157"/>
+      <c r="D6" s="157" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="158"/>
-      <c r="F6" s="159" t="s">
+      <c r="E6" s="157"/>
+      <c r="F6" s="158" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="162"/>
-      <c r="B7" s="154" t="s">
+      <c r="A7" s="161"/>
+      <c r="B7" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="154" t="s">
+      <c r="C7" s="153" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="154" t="s">
+      <c r="D7" s="153" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="154" t="s">
+      <c r="E7" s="153" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="160"/>
+      <c r="F7" s="159"/>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -10679,13 +10809,13 @@
       <c r="B16" s="51">
         <v>3011</v>
       </c>
-      <c r="C16" s="147">
+      <c r="C16" s="146">
         <v>77.2</v>
       </c>
       <c r="D16" s="51">
         <v>890</v>
       </c>
-      <c r="E16" s="147">
+      <c r="E16" s="146">
         <v>22.8</v>
       </c>
       <c r="F16" s="53">
@@ -10739,18 +10869,18 @@
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A20" s="157" t="s">
+      <c r="A20" s="156" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="157"/>
-      <c r="C20" s="157"/>
-      <c r="D20" s="157"/>
-      <c r="E20" s="157"/>
-      <c r="F20" s="157"/>
-      <c r="G20" s="157"/>
-      <c r="H20" s="157"/>
-      <c r="I20" s="157"/>
-      <c r="J20" s="157"/>
+      <c r="B20" s="156"/>
+      <c r="C20" s="156"/>
+      <c r="D20" s="156"/>
+      <c r="E20" s="156"/>
+      <c r="F20" s="156"/>
+      <c r="G20" s="156"/>
+      <c r="H20" s="156"/>
+      <c r="I20" s="156"/>
+      <c r="J20" s="156"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
@@ -10763,8 +10893,8 @@
       <c r="F21" s="18"/>
       <c r="G21" s="18"/>
       <c r="H21" s="18"/>
-      <c r="I21" s="148"/>
-      <c r="J21" s="148"/>
+      <c r="I21" s="147"/>
+      <c r="J21" s="147"/>
     </row>
     <row r="22" spans="1:10">
       <c r="A22" s="5" t="s">
@@ -10777,8 +10907,8 @@
       <c r="F22" s="18"/>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
-      <c r="I22" s="148"/>
-      <c r="J22" s="148"/>
+      <c r="I22" s="147"/>
+      <c r="J22" s="147"/>
     </row>
     <row r="23" spans="1:10">
       <c r="A23" s="5" t="s">
@@ -10791,8 +10921,8 @@
       <c r="F23" s="18"/>
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
-      <c r="I23" s="148"/>
-      <c r="J23" s="148"/>
+      <c r="I23" s="147"/>
+      <c r="J23" s="147"/>
     </row>
     <row r="24" spans="1:10">
       <c r="A24" s="5" t="s">
@@ -10805,22 +10935,22 @@
       <c r="F24" s="18"/>
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
-      <c r="I24" s="148"/>
-      <c r="J24" s="148"/>
+      <c r="I24" s="147"/>
+      <c r="J24" s="147"/>
     </row>
     <row r="25" spans="1:10" ht="24.5" customHeight="1">
-      <c r="A25" s="157" t="s">
+      <c r="A25" s="156" t="s">
         <v>219</v>
       </c>
-      <c r="B25" s="157"/>
-      <c r="C25" s="157"/>
-      <c r="D25" s="157"/>
-      <c r="E25" s="157"/>
-      <c r="F25" s="157"/>
-      <c r="G25" s="157"/>
-      <c r="H25" s="157"/>
-      <c r="I25" s="157"/>
-      <c r="J25" s="157"/>
+      <c r="B25" s="156"/>
+      <c r="C25" s="156"/>
+      <c r="D25" s="156"/>
+      <c r="E25" s="156"/>
+      <c r="F25" s="156"/>
+      <c r="G25" s="156"/>
+      <c r="H25" s="156"/>
+      <c r="I25" s="156"/>
+      <c r="J25" s="156"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="5"/>
@@ -10896,21 +11026,21 @@
     <row r="5" spans="1:11" ht="15" thickBot="1"/>
     <row r="6" spans="1:11" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="164" t="s">
+      <c r="H6" s="163" t="s">
         <v>68</v>
       </c>
     </row>
@@ -10928,9 +11058,9 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
-      <c r="H7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
+      <c r="H7" s="164"/>
     </row>
     <row r="8" spans="1:11" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -11288,7 +11418,7 @@
       <c r="F20" s="75">
         <v>3901</v>
       </c>
-      <c r="G20" s="149" t="s">
+      <c r="G20" s="148" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="72">
@@ -11316,7 +11446,7 @@
       <c r="F21" s="58">
         <v>32422</v>
       </c>
-      <c r="G21" s="151" t="s">
+      <c r="G21" s="150" t="s">
         <v>9</v>
       </c>
       <c r="H21" s="60"/>
@@ -11459,18 +11589,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>223</v>
       </c>
     </row>
@@ -11488,8 +11618,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -11811,7 +11941,7 @@
       <c r="F20" s="51">
         <v>891</v>
       </c>
-      <c r="G20" s="152">
+      <c r="G20" s="151">
         <v>100</v>
       </c>
       <c r="H20" s="33"/>
@@ -11885,18 +12015,18 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24.5" customHeight="1">
-      <c r="A27" s="157" t="s">
+      <c r="A27" s="156" t="s">
         <v>246</v>
       </c>
-      <c r="B27" s="157"/>
-      <c r="C27" s="157"/>
-      <c r="D27" s="157"/>
-      <c r="E27" s="157"/>
-      <c r="F27" s="157"/>
-      <c r="G27" s="157"/>
-      <c r="H27" s="157"/>
-      <c r="I27" s="157"/>
-      <c r="J27" s="157"/>
+      <c r="B27" s="156"/>
+      <c r="C27" s="156"/>
+      <c r="D27" s="156"/>
+      <c r="E27" s="156"/>
+      <c r="F27" s="156"/>
+      <c r="G27" s="156"/>
+      <c r="H27" s="156"/>
+      <c r="I27" s="156"/>
+      <c r="J27" s="156"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -11968,18 +12098,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>247</v>
       </c>
     </row>
@@ -11997,8 +12127,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -12320,7 +12450,7 @@
       <c r="F20" s="51">
         <v>1958</v>
       </c>
-      <c r="G20" s="152">
+      <c r="G20" s="151">
         <v>100</v>
       </c>
       <c r="H20" s="33"/>
@@ -12462,18 +12592,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="16" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>70</v>
       </c>
     </row>
@@ -12491,8 +12621,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -12513,7 +12643,7 @@
       <c r="F8" s="13">
         <v>15</v>
       </c>
-      <c r="G8" s="150">
+      <c r="G8" s="149">
         <v>2.2999999999999998</v>
       </c>
       <c r="H8" s="35"/>
@@ -12968,18 +13098,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="163" t="s">
+      <c r="B6" s="162" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="163"/>
-      <c r="D6" s="163" t="s">
+      <c r="C6" s="162"/>
+      <c r="D6" s="162" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="163"/>
-      <c r="F6" s="164" t="s">
+      <c r="E6" s="162"/>
+      <c r="F6" s="163" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="164" t="s">
+      <c r="G6" s="163" t="s">
         <v>71</v>
       </c>
     </row>
@@ -12997,8 +13127,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="165"/>
-      <c r="G7" s="165"/>
+      <c r="F7" s="164"/>
+      <c r="G7" s="164"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -13332,7 +13462,7 @@
       <c r="F20" s="51">
         <v>1455</v>
       </c>
-      <c r="G20" s="152">
+      <c r="G20" s="151">
         <v>100</v>
       </c>
       <c r="H20" s="35"/>

</xml_diff>

<commit_message>
add regional civil society
</commit_message>
<xml_diff>
--- a/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
+++ b/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28308"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19540" tabRatio="971" firstSheet="7" activeTab="18"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21940" tabRatio="971" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="948" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="257">
   <si>
     <t>UK</t>
   </si>
@@ -1391,7 +1391,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1400,6 +1400,7 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1844,6 +1845,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -1856,12 +1863,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1890,7 +1891,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="20">
+  <cellStyles count="21">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1907,6 +1908,7 @@
     <cellStyle name="Followed Hyperlink" xfId="17" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4037,74 +4039,74 @@
       <c r="X5" s="135"/>
     </row>
     <row r="6" spans="1:24" ht="42.5" customHeight="1">
-      <c r="A6" s="167" t="s">
+      <c r="A6" s="169" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="167"/>
-      <c r="C6" s="165" t="s">
+      <c r="B6" s="169"/>
+      <c r="C6" s="167" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="165" t="s">
+      <c r="D6" s="167" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="165" t="s">
+      <c r="E6" s="167" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="165" t="s">
+      <c r="F6" s="167" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="165" t="s">
+      <c r="G6" s="167" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="165" t="s">
+      <c r="H6" s="167" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="165" t="s">
+      <c r="I6" s="167" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="165" t="s">
+      <c r="J6" s="167" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="165" t="s">
+      <c r="K6" s="167" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="169"/>
-      <c r="O6" s="169"/>
-      <c r="P6" s="170"/>
-      <c r="Q6" s="170"/>
-      <c r="R6" s="170"/>
-      <c r="S6" s="170"/>
-      <c r="T6" s="170"/>
-      <c r="U6" s="170"/>
-      <c r="V6" s="170"/>
-      <c r="W6" s="170"/>
-      <c r="X6" s="170"/>
+      <c r="N6" s="166"/>
+      <c r="O6" s="166"/>
+      <c r="P6" s="165"/>
+      <c r="Q6" s="165"/>
+      <c r="R6" s="165"/>
+      <c r="S6" s="165"/>
+      <c r="T6" s="165"/>
+      <c r="U6" s="165"/>
+      <c r="V6" s="165"/>
+      <c r="W6" s="165"/>
+      <c r="X6" s="165"/>
     </row>
     <row r="7" spans="1:24" ht="21" customHeight="1" thickBot="1">
-      <c r="A7" s="168"/>
-      <c r="B7" s="168"/>
-      <c r="C7" s="166"/>
-      <c r="D7" s="166"/>
-      <c r="E7" s="166"/>
-      <c r="F7" s="166"/>
-      <c r="G7" s="166"/>
-      <c r="H7" s="166"/>
-      <c r="I7" s="166"/>
-      <c r="J7" s="166"/>
-      <c r="K7" s="166"/>
+      <c r="A7" s="170"/>
+      <c r="B7" s="170"/>
+      <c r="C7" s="168"/>
+      <c r="D7" s="168"/>
+      <c r="E7" s="168"/>
+      <c r="F7" s="168"/>
+      <c r="G7" s="168"/>
+      <c r="H7" s="168"/>
+      <c r="I7" s="168"/>
+      <c r="J7" s="168"/>
+      <c r="K7" s="168"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
-      <c r="N7" s="169"/>
-      <c r="O7" s="169"/>
-      <c r="P7" s="170"/>
-      <c r="Q7" s="170"/>
-      <c r="R7" s="170"/>
-      <c r="S7" s="170"/>
-      <c r="T7" s="170"/>
-      <c r="U7" s="170"/>
-      <c r="V7" s="170"/>
-      <c r="W7" s="170"/>
-      <c r="X7" s="170"/>
+      <c r="N7" s="166"/>
+      <c r="O7" s="166"/>
+      <c r="P7" s="165"/>
+      <c r="Q7" s="165"/>
+      <c r="R7" s="165"/>
+      <c r="S7" s="165"/>
+      <c r="T7" s="165"/>
+      <c r="U7" s="165"/>
+      <c r="V7" s="165"/>
+      <c r="W7" s="165"/>
+      <c r="X7" s="165"/>
     </row>
     <row r="8" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="61" t="s">
@@ -4781,16 +4783,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="T6:T7"/>
-    <mergeCell ref="U6:U7"/>
-    <mergeCell ref="V6:V7"/>
-    <mergeCell ref="W6:W7"/>
-    <mergeCell ref="X6:X7"/>
-    <mergeCell ref="N6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="Q6:Q7"/>
-    <mergeCell ref="R6:R7"/>
-    <mergeCell ref="S6:S7"/>
     <mergeCell ref="A28:J28"/>
     <mergeCell ref="K6:K7"/>
     <mergeCell ref="A6:B7"/>
@@ -4802,6 +4794,16 @@
     <mergeCell ref="I6:I7"/>
     <mergeCell ref="J6:J7"/>
     <mergeCell ref="C6:C7"/>
+    <mergeCell ref="N6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="Q6:Q7"/>
+    <mergeCell ref="R6:R7"/>
+    <mergeCell ref="S6:S7"/>
+    <mergeCell ref="T6:T7"/>
+    <mergeCell ref="U6:U7"/>
+    <mergeCell ref="V6:V7"/>
+    <mergeCell ref="W6:W7"/>
+    <mergeCell ref="X6:X7"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="K1" location="Contents!A1" display="Back to contents"/>
@@ -7547,7 +7549,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -10984,7 +10986,7 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -11185,10 +11187,10 @@
         <v>78.400000000000006</v>
       </c>
       <c r="D12" s="16">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12" s="37">
-        <v>21.3</v>
+        <v>21.6</v>
       </c>
       <c r="F12" s="40">
         <v>268</v>
@@ -11418,8 +11420,8 @@
       <c r="F20" s="75">
         <v>3901</v>
       </c>
-      <c r="G20" s="148" t="s">
-        <v>9</v>
+      <c r="G20" s="148">
+        <v>100</v>
       </c>
       <c r="H20" s="72">
         <v>12</v>
@@ -11446,9 +11448,7 @@
       <c r="F21" s="58">
         <v>32422</v>
       </c>
-      <c r="G21" s="150" t="s">
-        <v>9</v>
-      </c>
+      <c r="G21" s="150"/>
       <c r="H21" s="60"/>
       <c r="I21" s="33"/>
       <c r="K21" s="33"/>
@@ -11912,10 +11912,10 @@
       <c r="E19" s="37" t="s">
         <v>22</v>
       </c>
-      <c r="F19" s="16" t="s">
-        <v>22</v>
-      </c>
-      <c r="G19" s="17" t="s">
+      <c r="F19" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="37" t="s">
         <v>22</v>
       </c>
       <c r="H19" s="33"/>
@@ -12241,10 +12241,10 @@
         <v>66.8</v>
       </c>
       <c r="D12" s="16">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E12" s="37">
-        <v>32.5</v>
+        <v>33.200000000000003</v>
       </c>
       <c r="F12" s="16">
         <v>118</v>

</xml_diff>

<commit_message>
backup refactoring - passing
</commit_message>
<xml_diff>
--- a/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
+++ b/DCMS_Sectors_Economic_Estimates_Employment_2016_tables_2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28308"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21940" tabRatio="971" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="19540" tabRatio="971" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Contents" sheetId="38" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="946" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="954" uniqueCount="257">
   <si>
     <t>UK</t>
   </si>
@@ -1253,7 +1253,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -1390,8 +1390,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1400,6 +1409,8 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1417,7 +1428,7 @@
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" quotePrefix="1" applyFont="1"/>
@@ -1818,6 +1829,7 @@
     </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1891,7 +1903,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="23">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1909,6 +1921,8 @@
     <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Hyperlink 2" xfId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2829,7 +2843,9 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -3181,18 +3197,18 @@
     <row r="5" spans="1:11" ht="15" thickBot="1"/>
     <row r="6" spans="1:11" ht="16" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>73</v>
       </c>
     </row>
@@ -3210,8 +3226,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:11" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -3295,17 +3311,17 @@
       <c r="A11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B11" s="16">
-        <v>36</v>
-      </c>
-      <c r="C11" s="37">
-        <v>86.1</v>
-      </c>
-      <c r="D11" s="16">
-        <v>6</v>
-      </c>
-      <c r="E11" s="37">
-        <v>13.9</v>
+      <c r="B11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="37" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="37" t="s">
+        <v>22</v>
       </c>
       <c r="F11" s="16">
         <v>42</v>
@@ -3657,7 +3673,9 @@
   </sheetPr>
   <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -4039,74 +4057,74 @@
       <c r="X5" s="135"/>
     </row>
     <row r="6" spans="1:24" ht="42.5" customHeight="1">
-      <c r="A6" s="169" t="s">
+      <c r="A6" s="170" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="169"/>
-      <c r="C6" s="167" t="s">
+      <c r="B6" s="170"/>
+      <c r="C6" s="168" t="s">
         <v>231</v>
       </c>
-      <c r="D6" s="167" t="s">
+      <c r="D6" s="168" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="167" t="s">
+      <c r="E6" s="168" t="s">
         <v>3</v>
       </c>
-      <c r="F6" s="167" t="s">
+      <c r="F6" s="168" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="167" t="s">
+      <c r="G6" s="168" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="167" t="s">
+      <c r="H6" s="168" t="s">
         <v>6</v>
       </c>
-      <c r="I6" s="167" t="s">
+      <c r="I6" s="168" t="s">
         <v>7</v>
       </c>
-      <c r="J6" s="167" t="s">
+      <c r="J6" s="168" t="s">
         <v>47</v>
       </c>
-      <c r="K6" s="167" t="s">
+      <c r="K6" s="168" t="s">
         <v>48</v>
       </c>
-      <c r="N6" s="166"/>
-      <c r="O6" s="166"/>
-      <c r="P6" s="165"/>
-      <c r="Q6" s="165"/>
-      <c r="R6" s="165"/>
-      <c r="S6" s="165"/>
-      <c r="T6" s="165"/>
-      <c r="U6" s="165"/>
-      <c r="V6" s="165"/>
-      <c r="W6" s="165"/>
-      <c r="X6" s="165"/>
+      <c r="N6" s="167"/>
+      <c r="O6" s="167"/>
+      <c r="P6" s="166"/>
+      <c r="Q6" s="166"/>
+      <c r="R6" s="166"/>
+      <c r="S6" s="166"/>
+      <c r="T6" s="166"/>
+      <c r="U6" s="166"/>
+      <c r="V6" s="166"/>
+      <c r="W6" s="166"/>
+      <c r="X6" s="166"/>
     </row>
     <row r="7" spans="1:24" ht="21" customHeight="1" thickBot="1">
-      <c r="A7" s="170"/>
-      <c r="B7" s="170"/>
-      <c r="C7" s="168"/>
-      <c r="D7" s="168"/>
-      <c r="E7" s="168"/>
-      <c r="F7" s="168"/>
-      <c r="G7" s="168"/>
-      <c r="H7" s="168"/>
-      <c r="I7" s="168"/>
-      <c r="J7" s="168"/>
-      <c r="K7" s="168"/>
+      <c r="A7" s="171"/>
+      <c r="B7" s="171"/>
+      <c r="C7" s="169"/>
+      <c r="D7" s="169"/>
+      <c r="E7" s="169"/>
+      <c r="F7" s="169"/>
+      <c r="G7" s="169"/>
+      <c r="H7" s="169"/>
+      <c r="I7" s="169"/>
+      <c r="J7" s="169"/>
+      <c r="K7" s="169"/>
       <c r="L7" s="35"/>
       <c r="M7" s="35"/>
-      <c r="N7" s="166"/>
-      <c r="O7" s="166"/>
-      <c r="P7" s="165"/>
-      <c r="Q7" s="165"/>
-      <c r="R7" s="165"/>
-      <c r="S7" s="165"/>
-      <c r="T7" s="165"/>
-      <c r="U7" s="165"/>
-      <c r="V7" s="165"/>
-      <c r="W7" s="165"/>
-      <c r="X7" s="165"/>
+      <c r="N7" s="167"/>
+      <c r="O7" s="167"/>
+      <c r="P7" s="166"/>
+      <c r="Q7" s="166"/>
+      <c r="R7" s="166"/>
+      <c r="S7" s="166"/>
+      <c r="T7" s="166"/>
+      <c r="U7" s="166"/>
+      <c r="V7" s="166"/>
+      <c r="W7" s="166"/>
+      <c r="X7" s="166"/>
     </row>
     <row r="8" spans="1:24" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A8" s="61" t="s">
@@ -4768,18 +4786,18 @@
       </c>
     </row>
     <row r="28" spans="1:24" ht="29.75" customHeight="1">
-      <c r="A28" s="156" t="s">
+      <c r="A28" s="157" t="s">
         <v>246</v>
       </c>
-      <c r="B28" s="156"/>
-      <c r="C28" s="156"/>
-      <c r="D28" s="156"/>
-      <c r="E28" s="156"/>
-      <c r="F28" s="156"/>
-      <c r="G28" s="156"/>
-      <c r="H28" s="156"/>
-      <c r="I28" s="156"/>
-      <c r="J28" s="156"/>
+      <c r="B28" s="157"/>
+      <c r="C28" s="157"/>
+      <c r="D28" s="157"/>
+      <c r="E28" s="157"/>
+      <c r="F28" s="157"/>
+      <c r="G28" s="157"/>
+      <c r="H28" s="157"/>
+      <c r="I28" s="157"/>
+      <c r="J28" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="21">
@@ -4886,68 +4904,68 @@
       <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:18" s="76" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
-      <c r="B6" s="175" t="s">
+      <c r="B6" s="176" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="175"/>
-      <c r="D6" s="175"/>
-      <c r="E6" s="175"/>
-      <c r="F6" s="175"/>
-      <c r="G6" s="175" t="s">
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="176" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="175"/>
-      <c r="I6" s="175"/>
-      <c r="J6" s="175"/>
-      <c r="K6" s="175"/>
-      <c r="L6" s="175" t="s">
+      <c r="H6" s="176"/>
+      <c r="I6" s="176"/>
+      <c r="J6" s="176"/>
+      <c r="K6" s="176"/>
+      <c r="L6" s="176" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="175"/>
-      <c r="N6" s="175"/>
-      <c r="O6" s="175"/>
-      <c r="P6" s="175"/>
+      <c r="M6" s="176"/>
+      <c r="N6" s="176"/>
+      <c r="O6" s="176"/>
+      <c r="P6" s="176"/>
     </row>
     <row r="7" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="176" t="s">
+      <c r="A7" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="171" t="s">
+      <c r="B7" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="C7" s="171"/>
-      <c r="D7" s="171" t="s">
+      <c r="C7" s="172"/>
+      <c r="D7" s="172" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="171"/>
-      <c r="F7" s="172" t="s">
+      <c r="E7" s="172"/>
+      <c r="F7" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="171" t="s">
+      <c r="G7" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="171"/>
-      <c r="I7" s="171" t="s">
+      <c r="H7" s="172"/>
+      <c r="I7" s="172" t="s">
         <v>77</v>
       </c>
-      <c r="J7" s="171"/>
-      <c r="K7" s="172" t="s">
+      <c r="J7" s="172"/>
+      <c r="K7" s="173" t="s">
         <v>19</v>
       </c>
-      <c r="L7" s="171" t="s">
+      <c r="L7" s="172" t="s">
         <v>76</v>
       </c>
-      <c r="M7" s="171"/>
-      <c r="N7" s="171" t="s">
+      <c r="M7" s="172"/>
+      <c r="N7" s="172" t="s">
         <v>77</v>
       </c>
-      <c r="O7" s="171"/>
-      <c r="P7" s="172" t="s">
+      <c r="O7" s="172"/>
+      <c r="P7" s="173" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A8" s="177"/>
+      <c r="A8" s="178"/>
       <c r="B8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4960,7 +4978,7 @@
       <c r="E8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="173"/>
+      <c r="F8" s="174"/>
       <c r="G8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4973,7 +4991,7 @@
       <c r="J8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="K8" s="173"/>
+      <c r="K8" s="174"/>
       <c r="L8" s="124" t="s">
         <v>20</v>
       </c>
@@ -4986,7 +5004,7 @@
       <c r="O8" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="P8" s="173"/>
+      <c r="P8" s="174"/>
     </row>
     <row r="9" spans="1:18" ht="21" customHeight="1" thickTop="1">
       <c r="A9" s="87" t="s">
@@ -5461,15 +5479,15 @@
       <c r="H19" s="83"/>
     </row>
     <row r="20" spans="1:18">
-      <c r="A20" s="174" t="s">
+      <c r="A20" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="B20" s="174"/>
-      <c r="C20" s="174"/>
-      <c r="D20" s="174"/>
-      <c r="E20" s="174"/>
-      <c r="F20" s="174"/>
-      <c r="G20" s="174"/>
+      <c r="B20" s="175"/>
+      <c r="C20" s="175"/>
+      <c r="D20" s="175"/>
+      <c r="E20" s="175"/>
+      <c r="F20" s="175"/>
+      <c r="G20" s="175"/>
       <c r="H20" s="83"/>
     </row>
     <row r="21" spans="1:18">
@@ -5521,18 +5539,18 @@
       <c r="H24" s="83"/>
     </row>
     <row r="25" spans="1:18" ht="31.5" customHeight="1">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B25" s="156"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="156"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="156"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="157"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
     </row>
     <row r="26" spans="1:18">
       <c r="A26" s="82"/>
@@ -5623,18 +5641,18 @@
       </c>
     </row>
     <row r="6" spans="1:23" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="178" t="s">
+      <c r="B6" s="179" t="s">
         <v>78</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="179" t="s">
         <v>230</v>
       </c>
-      <c r="E6" s="178"/>
-      <c r="F6" s="172" t="s">
+      <c r="E6" s="179"/>
+      <c r="F6" s="173" t="s">
         <v>19</v>
       </c>
       <c r="G6" s="77" t="s">
@@ -5642,7 +5660,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="178"/>
       <c r="B7" s="124" t="s">
         <v>20</v>
       </c>
@@ -5655,7 +5673,7 @@
       <c r="E7" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="173"/>
+      <c r="F7" s="174"/>
     </row>
     <row r="8" spans="1:23" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="87" t="s">
@@ -5863,14 +5881,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="174" t="s">
+      <c r="A19" s="175" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="174"/>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -5913,18 +5931,18 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="30.5" customHeight="1">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -6015,33 +6033,33 @@
       <c r="P5" s="80"/>
     </row>
     <row r="6" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="179" t="s">
+      <c r="B6" s="180" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="179"/>
-      <c r="D6" s="179"/>
-      <c r="E6" s="179"/>
-      <c r="F6" s="179"/>
-      <c r="G6" s="179" t="s">
+      <c r="C6" s="180"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="180"/>
+      <c r="F6" s="180"/>
+      <c r="G6" s="180" t="s">
         <v>18</v>
       </c>
-      <c r="H6" s="179"/>
-      <c r="I6" s="179"/>
-      <c r="J6" s="179"/>
-      <c r="K6" s="179"/>
-      <c r="L6" s="179" t="s">
+      <c r="H6" s="180"/>
+      <c r="I6" s="180"/>
+      <c r="J6" s="180"/>
+      <c r="K6" s="180"/>
+      <c r="L6" s="180" t="s">
         <v>49</v>
       </c>
-      <c r="M6" s="179"/>
-      <c r="N6" s="179"/>
-      <c r="O6" s="179"/>
-      <c r="P6" s="179"/>
+      <c r="M6" s="180"/>
+      <c r="N6" s="180"/>
+      <c r="O6" s="180"/>
+      <c r="P6" s="180"/>
     </row>
     <row r="7" spans="1:18" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="178"/>
       <c r="B7" s="96" t="s">
         <v>79</v>
       </c>
@@ -6553,15 +6571,15 @@
       <c r="H18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="174" t="s">
+      <c r="A19" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="174"/>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
-      <c r="G19" s="174"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
+      <c r="G19" s="175"/>
       <c r="H19" s="83"/>
     </row>
     <row r="20" spans="1:10">
@@ -6613,18 +6631,18 @@
       <c r="H23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="27" customHeight="1">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -7034,15 +7052,15 @@
       <c r="H17" s="83"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="174" t="s">
+      <c r="A18" s="175" t="s">
         <v>92</v>
       </c>
-      <c r="B18" s="174"/>
-      <c r="C18" s="174"/>
-      <c r="D18" s="174"/>
-      <c r="E18" s="174"/>
-      <c r="F18" s="174"/>
-      <c r="G18" s="174"/>
+      <c r="B18" s="175"/>
+      <c r="C18" s="175"/>
+      <c r="D18" s="175"/>
+      <c r="E18" s="175"/>
+      <c r="F18" s="175"/>
+      <c r="G18" s="175"/>
       <c r="H18" s="83"/>
     </row>
     <row r="19" spans="1:10">
@@ -7106,18 +7124,18 @@
       <c r="H23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="25.25" customHeight="1">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="157" t="s">
         <v>249</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82" t="s">
@@ -7213,18 +7231,18 @@
       <c r="F5" s="80"/>
     </row>
     <row r="6" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="178" t="s">
+      <c r="B6" s="179" t="s">
         <v>89</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="179" t="s">
         <v>90</v>
       </c>
-      <c r="E6" s="178"/>
-      <c r="F6" s="172" t="s">
+      <c r="E6" s="179"/>
+      <c r="F6" s="173" t="s">
         <v>19</v>
       </c>
       <c r="I6" s="77" t="s">
@@ -7232,7 +7250,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="178"/>
       <c r="B7" s="124" t="s">
         <v>20</v>
       </c>
@@ -7245,7 +7263,7 @@
       <c r="E7" s="124" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="173"/>
+      <c r="F7" s="174"/>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="87" t="s">
@@ -7457,14 +7475,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="174" t="s">
+      <c r="A19" s="175" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="174"/>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -7507,18 +7525,18 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="27" customHeight="1">
-      <c r="A24" s="156" t="s">
+      <c r="A24" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B24" s="156"/>
-      <c r="C24" s="156"/>
-      <c r="D24" s="156"/>
-      <c r="E24" s="156"/>
-      <c r="F24" s="156"/>
-      <c r="G24" s="156"/>
-      <c r="H24" s="156"/>
-      <c r="I24" s="156"/>
-      <c r="J24" s="156"/>
+      <c r="B24" s="157"/>
+      <c r="C24" s="157"/>
+      <c r="D24" s="157"/>
+      <c r="E24" s="157"/>
+      <c r="F24" s="157"/>
+      <c r="G24" s="157"/>
+      <c r="H24" s="157"/>
+      <c r="I24" s="157"/>
+      <c r="J24" s="157"/>
     </row>
     <row r="25" spans="1:10">
       <c r="A25" s="82"/>
@@ -7599,27 +7617,27 @@
       <c r="F5" s="121"/>
     </row>
     <row r="6" spans="1:14" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="176" t="s">
+      <c r="A6" s="177" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="178" t="s">
+      <c r="B6" s="179" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="178"/>
-      <c r="D6" s="178" t="s">
+      <c r="C6" s="179"/>
+      <c r="D6" s="179" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="178"/>
-      <c r="F6" s="178" t="s">
+      <c r="E6" s="179"/>
+      <c r="F6" s="179" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="178"/>
+      <c r="G6" s="179"/>
       <c r="I6" s="77" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="177"/>
+      <c r="A7" s="178"/>
       <c r="B7" s="124" t="s">
         <v>211</v>
       </c>
@@ -7922,14 +7940,14 @@
       <c r="F18" s="83"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="174" t="s">
+      <c r="A19" s="175" t="s">
         <v>40</v>
       </c>
-      <c r="B19" s="174"/>
-      <c r="C19" s="174"/>
-      <c r="D19" s="174"/>
-      <c r="E19" s="174"/>
-      <c r="F19" s="174"/>
+      <c r="B19" s="175"/>
+      <c r="C19" s="175"/>
+      <c r="D19" s="175"/>
+      <c r="E19" s="175"/>
+      <c r="F19" s="175"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="82" t="s">
@@ -7972,29 +7990,29 @@
       <c r="F23" s="83"/>
     </row>
     <row r="24" spans="1:10" ht="28.5" customHeight="1">
-      <c r="A24" s="174" t="s">
+      <c r="A24" s="175" t="s">
         <v>217</v>
       </c>
-      <c r="B24" s="174"/>
-      <c r="C24" s="174"/>
-      <c r="D24" s="174"/>
-      <c r="E24" s="174"/>
-      <c r="F24" s="174"/>
-      <c r="G24" s="174"/>
+      <c r="B24" s="175"/>
+      <c r="C24" s="175"/>
+      <c r="D24" s="175"/>
+      <c r="E24" s="175"/>
+      <c r="F24" s="175"/>
+      <c r="G24" s="175"/>
     </row>
     <row r="25" spans="1:10" ht="17.75" customHeight="1">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="157" t="s">
         <v>249</v>
       </c>
-      <c r="B25" s="156"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="156"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="156"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="157"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -8513,18 +8531,18 @@
       <c r="J20" s="18"/>
     </row>
     <row r="21" spans="1:13" ht="29.25" customHeight="1">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="157" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="156"/>
-      <c r="C21" s="156"/>
-      <c r="D21" s="156"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="156"/>
-      <c r="G21" s="156"/>
-      <c r="H21" s="156"/>
-      <c r="I21" s="156"/>
-      <c r="J21" s="156"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="5" t="s">
@@ -8569,18 +8587,18 @@
       <c r="J24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="28.5" customHeight="1">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B25" s="156"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="156"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="156"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="157"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="5" t="s">
@@ -9852,15 +9870,15 @@
       <c r="G77" s="83"/>
     </row>
     <row r="78" spans="1:7" ht="27.5" customHeight="1">
-      <c r="A78" s="174" t="s">
+      <c r="A78" s="175" t="s">
         <v>250</v>
       </c>
-      <c r="B78" s="174"/>
-      <c r="C78" s="174"/>
-      <c r="D78" s="174"/>
-      <c r="E78" s="174"/>
-      <c r="F78" s="174"/>
-      <c r="G78" s="174"/>
+      <c r="B78" s="175"/>
+      <c r="C78" s="175"/>
+      <c r="D78" s="175"/>
+      <c r="E78" s="175"/>
+      <c r="F78" s="175"/>
+      <c r="G78" s="175"/>
     </row>
     <row r="79" spans="1:7">
       <c r="A79" s="82" t="s">
@@ -9907,18 +9925,18 @@
       <c r="G82" s="83"/>
     </row>
     <row r="83" spans="1:10">
-      <c r="A83" s="156" t="s">
+      <c r="A83" s="157" t="s">
         <v>245</v>
       </c>
-      <c r="B83" s="156"/>
-      <c r="C83" s="156"/>
-      <c r="D83" s="156"/>
-      <c r="E83" s="156"/>
-      <c r="F83" s="156"/>
-      <c r="G83" s="156"/>
-      <c r="H83" s="156"/>
-      <c r="I83" s="156"/>
-      <c r="J83" s="156"/>
+      <c r="B83" s="157"/>
+      <c r="C83" s="157"/>
+      <c r="D83" s="157"/>
+      <c r="E83" s="157"/>
+      <c r="F83" s="157"/>
+      <c r="G83" s="157"/>
+      <c r="H83" s="157"/>
+      <c r="I83" s="157"/>
+      <c r="J83" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10394,18 +10412,18 @@
       <c r="Q20" s="33"/>
     </row>
     <row r="21" spans="1:17" ht="26.75" customHeight="1">
-      <c r="A21" s="156" t="s">
+      <c r="A21" s="157" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="156"/>
-      <c r="C21" s="156"/>
-      <c r="D21" s="156"/>
-      <c r="E21" s="156"/>
-      <c r="F21" s="156"/>
-      <c r="G21" s="156"/>
-      <c r="H21" s="156"/>
-      <c r="I21" s="156"/>
-      <c r="J21" s="156"/>
+      <c r="B21" s="157"/>
+      <c r="C21" s="157"/>
+      <c r="D21" s="157"/>
+      <c r="E21" s="157"/>
+      <c r="F21" s="157"/>
+      <c r="G21" s="157"/>
+      <c r="H21" s="157"/>
+      <c r="I21" s="157"/>
+      <c r="J21" s="157"/>
       <c r="L21" s="32"/>
       <c r="M21" s="32"/>
       <c r="N21" s="32"/>
@@ -10414,18 +10432,18 @@
       <c r="Q21" s="33"/>
     </row>
     <row r="22" spans="1:17" ht="29.25" customHeight="1">
-      <c r="A22" s="156" t="s">
+      <c r="A22" s="157" t="s">
         <v>244</v>
       </c>
-      <c r="B22" s="156"/>
-      <c r="C22" s="156"/>
-      <c r="D22" s="156"/>
-      <c r="E22" s="156"/>
-      <c r="F22" s="156"/>
-      <c r="G22" s="156"/>
-      <c r="H22" s="156"/>
-      <c r="I22" s="156"/>
-      <c r="J22" s="156"/>
+      <c r="B22" s="157"/>
+      <c r="C22" s="157"/>
+      <c r="D22" s="157"/>
+      <c r="E22" s="157"/>
+      <c r="F22" s="157"/>
+      <c r="G22" s="157"/>
+      <c r="H22" s="157"/>
+      <c r="I22" s="157"/>
+      <c r="J22" s="157"/>
       <c r="L22" s="32"/>
       <c r="M22" s="32"/>
       <c r="N22" s="32"/>
@@ -10597,23 +10615,23 @@
     </row>
     <row r="5" spans="1:9" ht="15" thickBot="1"/>
     <row r="6" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A6" s="160" t="s">
+      <c r="A6" s="161" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="157" t="s">
+      <c r="B6" s="158" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="157"/>
-      <c r="D6" s="157" t="s">
+      <c r="C6" s="158"/>
+      <c r="D6" s="158" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="157"/>
-      <c r="F6" s="158" t="s">
+      <c r="E6" s="158"/>
+      <c r="F6" s="159" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A7" s="161"/>
+      <c r="A7" s="162"/>
       <c r="B7" s="153" t="s">
         <v>20</v>
       </c>
@@ -10626,7 +10644,7 @@
       <c r="E7" s="153" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="159"/>
+      <c r="F7" s="160"/>
     </row>
     <row r="8" spans="1:9" ht="21" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -10871,18 +10889,18 @@
       <c r="H19" s="18"/>
     </row>
     <row r="20" spans="1:10" ht="24.75" customHeight="1">
-      <c r="A20" s="156" t="s">
+      <c r="A20" s="157" t="s">
         <v>254</v>
       </c>
-      <c r="B20" s="156"/>
-      <c r="C20" s="156"/>
-      <c r="D20" s="156"/>
-      <c r="E20" s="156"/>
-      <c r="F20" s="156"/>
-      <c r="G20" s="156"/>
-      <c r="H20" s="156"/>
-      <c r="I20" s="156"/>
-      <c r="J20" s="156"/>
+      <c r="B20" s="157"/>
+      <c r="C20" s="157"/>
+      <c r="D20" s="157"/>
+      <c r="E20" s="157"/>
+      <c r="F20" s="157"/>
+      <c r="G20" s="157"/>
+      <c r="H20" s="157"/>
+      <c r="I20" s="157"/>
+      <c r="J20" s="157"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="5" t="s">
@@ -10941,18 +10959,18 @@
       <c r="J24" s="147"/>
     </row>
     <row r="25" spans="1:10" ht="24.5" customHeight="1">
-      <c r="A25" s="156" t="s">
+      <c r="A25" s="157" t="s">
         <v>219</v>
       </c>
-      <c r="B25" s="156"/>
-      <c r="C25" s="156"/>
-      <c r="D25" s="156"/>
-      <c r="E25" s="156"/>
-      <c r="F25" s="156"/>
-      <c r="G25" s="156"/>
-      <c r="H25" s="156"/>
-      <c r="I25" s="156"/>
-      <c r="J25" s="156"/>
+      <c r="B25" s="157"/>
+      <c r="C25" s="157"/>
+      <c r="D25" s="157"/>
+      <c r="E25" s="157"/>
+      <c r="F25" s="157"/>
+      <c r="G25" s="157"/>
+      <c r="H25" s="157"/>
+      <c r="I25" s="157"/>
+      <c r="J25" s="157"/>
     </row>
     <row r="26" spans="1:10">
       <c r="A26" s="5"/>
@@ -10986,7 +11004,9 @@
   </sheetPr>
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -11028,21 +11048,21 @@
     <row r="5" spans="1:11" ht="15" thickBot="1"/>
     <row r="6" spans="1:11" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>69</v>
       </c>
-      <c r="H6" s="163" t="s">
+      <c r="H6" s="164" t="s">
         <v>68</v>
       </c>
     </row>
@@ -11060,9 +11080,9 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
-      <c r="H7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
+      <c r="H7" s="165"/>
     </row>
     <row r="8" spans="1:11" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -11412,7 +11432,7 @@
         <v>77.2</v>
       </c>
       <c r="D20" s="73">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="E20" s="74">
         <v>22.8</v>
@@ -11424,7 +11444,7 @@
         <v>100</v>
       </c>
       <c r="H20" s="72">
-        <v>12</v>
+        <v>12.1</v>
       </c>
       <c r="I20" s="33"/>
       <c r="K20" s="33"/>
@@ -11589,18 +11609,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>223</v>
       </c>
     </row>
@@ -11618,8 +11638,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -12015,18 +12035,18 @@
       </c>
     </row>
     <row r="27" spans="1:11" ht="24.5" customHeight="1">
-      <c r="A27" s="156" t="s">
+      <c r="A27" s="157" t="s">
         <v>246</v>
       </c>
-      <c r="B27" s="156"/>
-      <c r="C27" s="156"/>
-      <c r="D27" s="156"/>
-      <c r="E27" s="156"/>
-      <c r="F27" s="156"/>
-      <c r="G27" s="156"/>
-      <c r="H27" s="156"/>
-      <c r="I27" s="156"/>
-      <c r="J27" s="156"/>
+      <c r="B27" s="157"/>
+      <c r="C27" s="157"/>
+      <c r="D27" s="157"/>
+      <c r="E27" s="157"/>
+      <c r="F27" s="157"/>
+      <c r="G27" s="157"/>
+      <c r="H27" s="157"/>
+      <c r="I27" s="157"/>
+      <c r="J27" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -12098,18 +12118,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>247</v>
       </c>
     </row>
@@ -12127,8 +12147,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -12442,10 +12462,10 @@
         <v>65.5</v>
       </c>
       <c r="D20" s="51">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="E20" s="52">
-        <v>34.4</v>
+        <v>34.5</v>
       </c>
       <c r="F20" s="51">
         <v>1958</v>
@@ -12550,7 +12570,9 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="N11" sqref="N11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -12592,18 +12614,18 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="16" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>70</v>
       </c>
     </row>
@@ -12621,8 +12643,8 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
@@ -13054,9 +13076,11 @@
   <sheetPr codeName="Sheet8" enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
@@ -13098,20 +13122,21 @@
     <row r="5" spans="1:10" ht="15" thickBot="1"/>
     <row r="6" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A6" s="23"/>
-      <c r="B6" s="162" t="s">
+      <c r="B6" s="163" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="162"/>
-      <c r="D6" s="162" t="s">
+      <c r="C6" s="163"/>
+      <c r="D6" s="163" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="162"/>
-      <c r="F6" s="163" t="s">
+      <c r="E6" s="163"/>
+      <c r="F6" s="164" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="163" t="s">
+      <c r="G6" s="164" t="s">
         <v>71</v>
       </c>
+      <c r="J6" s="156"/>
     </row>
     <row r="7" spans="1:10" ht="42.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A7" s="23"/>
@@ -13127,24 +13152,24 @@
       <c r="E7" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="164"/>
-      <c r="G7" s="164"/>
+      <c r="F7" s="165"/>
+      <c r="G7" s="165"/>
     </row>
     <row r="8" spans="1:10" ht="20.5" customHeight="1" thickTop="1">
       <c r="A8" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="13">
-        <v>32</v>
-      </c>
-      <c r="C8" s="36">
-        <v>87.8</v>
-      </c>
-      <c r="D8" s="13">
-        <v>4</v>
-      </c>
-      <c r="E8" s="36">
-        <v>12.2</v>
+      <c r="B8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>22</v>
       </c>
       <c r="F8" s="13">
         <v>36</v>
@@ -13364,7 +13389,7 @@
       <c r="I16" s="35"/>
       <c r="J16" s="35"/>
     </row>
-    <row r="17" spans="1:11" ht="20.5" customHeight="1">
+    <row r="17" spans="1:15" ht="20.5" customHeight="1">
       <c r="A17" s="15" t="s">
         <v>35</v>
       </c>
@@ -13390,7 +13415,7 @@
       <c r="I17" s="35"/>
       <c r="J17" s="35"/>
     </row>
-    <row r="18" spans="1:11" ht="20.5" customHeight="1">
+    <row r="18" spans="1:15" ht="20.5" customHeight="1">
       <c r="A18" s="15" t="s">
         <v>36</v>
       </c>
@@ -13416,7 +13441,7 @@
       <c r="I18" s="35"/>
       <c r="J18" s="35"/>
     </row>
-    <row r="19" spans="1:11" s="42" customFormat="1" ht="20.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:15" s="42" customFormat="1" ht="20.5" customHeight="1" thickBot="1">
       <c r="A19" s="15" t="s">
         <v>37</v>
       </c>
@@ -13443,7 +13468,7 @@
       <c r="J19" s="35"/>
       <c r="K19"/>
     </row>
-    <row r="20" spans="1:11" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="20" spans="1:15" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A20" s="50" t="s">
         <v>38</v>
       </c>
@@ -13467,8 +13492,9 @@
       </c>
       <c r="H20" s="35"/>
       <c r="J20" s="35"/>
-    </row>
-    <row r="21" spans="1:11" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
+      <c r="O20" s="156"/>
+    </row>
+    <row r="21" spans="1:15" ht="20.5" customHeight="1" thickTop="1" thickBot="1">
       <c r="A21" s="54" t="s">
         <v>39</v>
       </c>
@@ -13491,7 +13517,7 @@
       <c r="H21" s="35"/>
       <c r="J21" s="35"/>
     </row>
-    <row r="22" spans="1:11" ht="8" customHeight="1" thickTop="1">
+    <row r="22" spans="1:15" ht="8" customHeight="1" thickTop="1">
       <c r="A22" s="5"/>
       <c r="B22" s="18"/>
       <c r="C22" s="18"/>
@@ -13501,7 +13527,7 @@
       <c r="G22" s="18"/>
       <c r="H22" s="35"/>
     </row>
-    <row r="23" spans="1:11">
+    <row r="23" spans="1:15">
       <c r="A23" s="4" t="s">
         <v>10</v>
       </c>
@@ -13513,7 +13539,7 @@
       <c r="G23" s="18"/>
       <c r="H23" s="18"/>
     </row>
-    <row r="24" spans="1:11">
+    <row r="24" spans="1:15">
       <c r="A24" s="5" t="s">
         <v>43</v>
       </c>
@@ -13525,7 +13551,7 @@
       <c r="G24" s="18"/>
       <c r="H24" s="18"/>
     </row>
-    <row r="25" spans="1:11">
+    <row r="25" spans="1:15">
       <c r="A25" s="5" t="s">
         <v>44</v>
       </c>
@@ -13537,12 +13563,12 @@
       <c r="G25" s="18"/>
       <c r="H25" s="18"/>
     </row>
-    <row r="26" spans="1:11">
+    <row r="26" spans="1:15">
       <c r="A26" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
+    <row r="27" spans="1:15">
       <c r="A27" s="5" t="s">
         <v>66</v>
       </c>

</xml_diff>